<commit_message>
updated subthemes through Birds
</commit_message>
<xml_diff>
--- a/subthemesCombo.xlsx
+++ b/subthemesCombo.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -591,7 +591,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Woolf</t>
+          <t>Virginia Woolf</t>
         </is>
       </c>
     </row>
@@ -608,7 +608,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Woolf</t>
+          <t>Virginia Woolf</t>
         </is>
       </c>
     </row>
@@ -625,7 +625,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Woolf</t>
+          <t>Virginia Woolf</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Woolf</t>
+          <t>Virginia Woolf</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AlcAdditional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AlcAdditional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AlcAdditional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AlcAdditional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AlcAdditional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -744,24 +744,24 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AlcAdditional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Decisions</t>
+          <t>Alcohol</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Difficult, and Uncertain Timing</t>
+          <t>Moderation and Tradeoffs</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Believe in Magic</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Inexplicable</t>
+          <t>Difficult, and Uncertain Timing</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -790,7 +790,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Regret</t>
+          <t>Inexplicable</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Power and Pain</t>
+          <t>Regret</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Life Changing But Slowly Develop</t>
+          <t>Power and Pain</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -841,12 +841,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Coin Flips</t>
+          <t>Life Changing But Slowly Develop</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Road Not Taken</t>
+          <t>Believe in Magic</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cognitive Dissonance</t>
+          <t>Coin Flips</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Compounding and Curtailing</t>
+          <t>Cognitive Dissonance</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Counterfactuals</t>
+          <t>Compounding and Curtailing</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Retrospective Logic</t>
+          <t>Counterfactuals</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -926,12 +926,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>External Pressure</t>
+          <t>Retrospective Logic</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Sophie's Choice</t>
+          <t>Road Not Taken</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Hair-Trigger</t>
+          <t>External Pressure</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Values and Incommensurables</t>
+          <t>Under the Gun</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -977,7 +977,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Partial Information</t>
+          <t>Values and Incommensurables</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -994,12 +994,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Ubiquity</t>
+          <t>Partial Information</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Card Players</t>
+          <t>Sophie's Choice</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Constrained or Wide Open</t>
+          <t>Ubiquity</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Solo or Multiple Deciders</t>
+          <t>Constrained or Wide Open</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Pattern Identification</t>
+          <t>Solo or Multiple Deciders</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Meaningfulness</t>
+          <t>Pattern Identification</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1079,12 +1079,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Rarely Final</t>
+          <t>Meaningfulness</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Decision Additional</t>
+          <t>Card Players</t>
         </is>
       </c>
     </row>
@@ -1096,12 +1096,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Inner Monologue</t>
+          <t>Rarely Final</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Decision Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1113,29 +1113,29 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Humanity's Advantage</t>
+          <t>Inner Monologue</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Decision Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Decisions</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Nature's Cycles</t>
+          <t>Humanity's Advantage</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ozymandias</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Humans Wreaking</t>
+          <t>Nature's Cycles</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Civilization Falls</t>
+          <t>Humans Wreaking</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Retribution</t>
+          <t>Civilization Falls</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Mighty</t>
+          <t>Retribution</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Flood at Port-Marley</t>
+          <t>Ozymandias</t>
         </is>
       </c>
     </row>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sudden</t>
+          <t>Mighty</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1232,7 +1232,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Widespread</t>
+          <t>Sudden</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Death and Sickness</t>
+          <t>Widespread</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Delayed Effects</t>
+          <t>Death and Sickness</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1283,12 +1283,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Social Strife</t>
+          <t>Delayed Effects</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>My Hometown</t>
+          <t>Flood at Port-Marley</t>
         </is>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Economic Pressure</t>
+          <t>Social Strife</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Foreseeability</t>
+          <t>Economic Pressure</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Anger</t>
+          <t>Foreseeability</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1351,12 +1351,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Deaths of Humans</t>
+          <t>Anger</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Saving Private Ryan</t>
+          <t>My Hometown</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Planned and Purposeful</t>
+          <t>Deaths of Humans</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Unilateral or Not</t>
+          <t>Planned and Purposeful</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Completely Wasteful</t>
+          <t>Unilateral or Not</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1419,12 +1419,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Rarely Final</t>
+          <t>Completely Wasteful</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Destruct Additional</t>
+          <t>Saving Private Ryan</t>
         </is>
       </c>
     </row>
@@ -1436,12 +1436,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Inner Monologue</t>
+          <t>Pandemics and Drugs</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Destruct Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1453,46 +1453,46 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Humanity's Advantage</t>
+          <t>Indiscriminate Destruction</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Destruct Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Work</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Workaholic</t>
+          <t>Entropy</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Citizen Kane</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Work</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Directing Others</t>
+          <t>Humans Cope</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Citizen Kane</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Responsibility</t>
+          <t>Workaholic</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Reputation</t>
+          <t>Directing Others</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1538,12 +1538,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Bosses</t>
+          <t>Responsibility</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Proud Mary</t>
+          <t>Citizen Kane</t>
         </is>
       </c>
     </row>
@@ -1555,12 +1555,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Job hopping</t>
+          <t>Reputation</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Proud Mary</t>
+          <t>Citizen Kane</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Reactive</t>
+          <t>Bosses</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Social Side</t>
+          <t>Job Hopping</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1606,12 +1606,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Manual Deterioration</t>
+          <t>Reactive</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Scrapers</t>
+          <t>Proud Mary</t>
         </is>
       </c>
     </row>
@@ -1623,12 +1623,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Piecework</t>
+          <t>Social Side</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Scrapers</t>
+          <t>Proud Mary</t>
         </is>
       </c>
     </row>
@@ -1640,12 +1640,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Little or No Education</t>
+          <t>Manual Deterioration</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Scrapers</t>
+          <t>Floor Scrapers</t>
         </is>
       </c>
     </row>
@@ -1657,12 +1657,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Attention to Detail</t>
+          <t>Piecework</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Scrapers</t>
+          <t>Floor Scrapers</t>
         </is>
       </c>
     </row>
@@ -1674,12 +1674,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Work vs. Career/Profession</t>
+          <t>Little or No Education</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Scrapers</t>
+          <t>Floor Scrapers</t>
         </is>
       </c>
     </row>
@@ -1691,12 +1691,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Attention to Detail</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Stopping by Woods</t>
+          <t>Floor Scrapers</t>
         </is>
       </c>
     </row>
@@ -1708,12 +1708,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Necessary</t>
+          <t>Work vs. Career/Profession</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Stopping by Woods</t>
+          <t>Floor Scrapers</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Father's Vocation</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Gig Economy</t>
+          <t>Necessary</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Not First Preference</t>
+          <t>Father's Vocation</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1776,12 +1776,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>Gig Economy</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Work Additional</t>
+          <t>Stopping by Woods</t>
         </is>
       </c>
     </row>
@@ -1793,12 +1793,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Labor, Task, Job, Career, Profession</t>
+          <t>Not First Preference</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Work Additional</t>
+          <t>Stopping by Woods</t>
         </is>
       </c>
     </row>
@@ -1810,12 +1810,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Vacations and Holidays</t>
+          <t>Money</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Work Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1827,46 +1827,46 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Unpredictable Journey</t>
+          <t>Labor, Task, Job, Career, Profession</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Work Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Work</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alarm Clocks </t>
+          <t>Vacations and Holidays</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Time Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Work</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Boredom and Loops </t>
+          <t>Unpredictable Journey</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Time Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Turn Back the Clock </t>
+          <t>Alarm Clocks</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Time Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1895,12 +1895,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t xml:space="preserve">One Direction </t>
+          <t>Boredom and Loops</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Time Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1912,12 +1912,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Passage of Time</t>
+          <t>Turn Back the Clock</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Time Bellili</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1929,12 +1929,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Time With the Family</t>
+          <t>One Direction</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Time Bellili</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -1946,12 +1946,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Punctuality</t>
+          <t>Passage of Time</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Time Bellili</t>
+          <t>Bellili Family</t>
         </is>
       </c>
     </row>
@@ -1963,12 +1963,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Integral to Commerce</t>
+          <t>Time With the Family</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Time Bellili</t>
+          <t>Bellili Family</t>
         </is>
       </c>
     </row>
@@ -1980,12 +1980,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Ample Time Suggests Leisure</t>
+          <t>Punctuality</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Time Coy</t>
+          <t>Bellili Family</t>
         </is>
       </c>
     </row>
@@ -1997,12 +1997,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Time Leads to Quality</t>
+          <t>Integral to Commerce</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Time Coy</t>
+          <t>Bellili Family</t>
         </is>
       </c>
     </row>
@@ -2014,12 +2014,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Carpe Diem</t>
+          <t>Ample Time Suggests Leisure</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Time Coy</t>
+          <t>Coy Mistress</t>
         </is>
       </c>
     </row>
@@ -2031,12 +2031,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Rate Time Passes Varies by Pleasure</t>
+          <t>Time Leads to Quality</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Time Coy</t>
+          <t>Coy Mistress</t>
         </is>
       </c>
     </row>
@@ -2048,12 +2048,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Never Stops</t>
+          <t>Carpe Diem</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Time Coy</t>
+          <t>Coy Mistress</t>
         </is>
       </c>
     </row>
@@ -2065,12 +2065,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Nature's Cycles</t>
+          <t>Rate Time Passes Varies by Pleasure</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Time Turn</t>
+          <t>Coy Mistress</t>
         </is>
       </c>
     </row>
@@ -2082,12 +2082,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Time and Religion</t>
+          <t>Never Stops</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Time Turn</t>
+          <t>Coy Mistress</t>
         </is>
       </c>
     </row>
@@ -2099,12 +2099,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t xml:space="preserve">A Lifetime </t>
+          <t>Nature's Cycles</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Time Turn</t>
+          <t>Turn Turn</t>
         </is>
       </c>
     </row>
@@ -2116,46 +2116,46 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t xml:space="preserve">To Act or Not to Act </t>
+          <t>Time and Religion</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Time Turn</t>
+          <t>Turn Turn</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Chance</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Non-Quantified Language</t>
+          <t>A Lifetime</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Chance Add</t>
+          <t>Turn Turn</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Chance</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Quantum Probability</t>
+          <t xml:space="preserve">To Act or Not to Act </t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Chance Add</t>
+          <t>Turn Turn</t>
         </is>
       </c>
     </row>
@@ -2167,12 +2167,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Risk Aversion</t>
+          <t>Non-Quantified Language</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Chance Add</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2184,12 +2184,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Randomness or Religion</t>
+          <t>Quantum Probability</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Chance Church</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2201,12 +2201,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Miracles and Saints</t>
+          <t>Risk Aversion</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Chance Church</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2218,12 +2218,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Reduce Chanciness</t>
+          <t>Randomness or Religion</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Chance Church</t>
+          <t>Quai St-Michel</t>
         </is>
       </c>
     </row>
@@ -2235,12 +2235,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Coincidence of Meeting</t>
+          <t>Miracles and Saints</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Chance Church</t>
+          <t>Quai St-Michel</t>
         </is>
       </c>
     </row>
@@ -2252,12 +2252,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Risk</t>
+          <t>Reduce Chanciness</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Chance Deer</t>
+          <t>Quai St-Michel</t>
         </is>
       </c>
     </row>
@@ -2269,12 +2269,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Nerves of Steel</t>
+          <t>Coincidence of Meeting</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Chance Deer</t>
+          <t>Quai St-Michel</t>
         </is>
       </c>
     </row>
@@ -2286,12 +2286,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Act Against the Odds</t>
+          <t>Risk</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Chance Deer</t>
+          <t>Deer Hunter</t>
         </is>
       </c>
     </row>
@@ -2303,12 +2303,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Entertainment Component</t>
+          <t>Nerves of Steel</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Chance Deer</t>
+          <t>Deer Hunter</t>
         </is>
       </c>
     </row>
@@ -2320,12 +2320,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Randomness of Events</t>
+          <t>Act Against the Odds</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Chance Hap</t>
+          <t>Deer Hunter</t>
         </is>
       </c>
     </row>
@@ -2337,12 +2337,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Good or Bad Luck</t>
+          <t>Entertainment Component</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Chance Hap</t>
+          <t>Deer Hunter</t>
         </is>
       </c>
     </row>
@@ -2354,12 +2354,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Opportunity</t>
+          <t>Randomness of Events</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Chance Hap</t>
+          <t>Hap</t>
         </is>
       </c>
     </row>
@@ -2371,12 +2371,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Good or Bad Luck</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Chance Hap</t>
+          <t>Hap</t>
         </is>
       </c>
     </row>
@@ -2388,12 +2388,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Bad Things Happen</t>
+          <t>Opportunity</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Chance Winner</t>
+          <t>Hap</t>
         </is>
       </c>
     </row>
@@ -2405,12 +2405,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Unknown Future</t>
+          <t>Probability</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Chance Winner</t>
+          <t>Hap</t>
         </is>
       </c>
     </row>
@@ -2422,46 +2422,46 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Physical or Person</t>
+          <t>Bad Things Happen</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Chance Winner</t>
+          <t>Winner Takes It</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Silence</t>
+          <t>Chance</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Silence Enables Communication</t>
+          <t>Unknown Future</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Silence Add</t>
+          <t>Winner Takes It</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Silence</t>
+          <t>Chance</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Out in Nature</t>
+          <t>Physical or Person</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Silence Add</t>
+          <t>Winner Takes It</t>
         </is>
       </c>
     </row>
@@ -2473,12 +2473,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Utter Silence of Outer Space</t>
+          <t>Silence Enables Communication</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Silence Add</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2490,12 +2490,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Deep Thought</t>
+          <t>Out in Nature</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Silence Add</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2507,12 +2507,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Anger or Disappointment</t>
+          <t>Utter Silence of Outer Space</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Silence Avril</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2524,12 +2524,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Introverted</t>
+          <t>Deep Thought</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Silence Avril</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2541,12 +2541,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Disapproval</t>
+          <t>Anger or Disappointment</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Silence Avril</t>
+          <t>Avril</t>
         </is>
       </c>
     </row>
@@ -2558,12 +2558,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Introverted</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Silence Bell Tolls</t>
+          <t>Avril</t>
         </is>
       </c>
     </row>
@@ -2575,12 +2575,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Reverence or Awe</t>
+          <t>Disapproval</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Silence Bell Tolls</t>
+          <t>Avril</t>
         </is>
       </c>
     </row>
@@ -2592,12 +2592,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Cessation</t>
+          <t>Death</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Silence Bell Tolls</t>
+          <t>Bell Tolls</t>
         </is>
       </c>
     </row>
@@ -2609,12 +2609,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Prayer</t>
+          <t>Reverence or Awe</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Silence Bell Tolls</t>
+          <t>Bell Tolls</t>
         </is>
       </c>
     </row>
@@ -2626,12 +2626,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Concealment</t>
+          <t>Cessation</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Silence Northwest</t>
+          <t>Bell Tolls</t>
         </is>
       </c>
     </row>
@@ -2643,12 +2643,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Authority</t>
+          <t>Prayer</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Silence Northwest</t>
+          <t>Bell Tolls</t>
         </is>
       </c>
     </row>
@@ -2660,12 +2660,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Hush</t>
+          <t>Concealment</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Silence Northwest</t>
+          <t>North by Northwest</t>
         </is>
       </c>
     </row>
@@ -2677,12 +2677,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Contrast to Conversation</t>
+          <t>Authority</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Silence Sounds</t>
+          <t>North by Northwest</t>
         </is>
       </c>
     </row>
@@ -2694,12 +2694,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Alienation and Depression</t>
+          <t>Hush</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Silence Sounds</t>
+          <t>North by Northwest</t>
         </is>
       </c>
     </row>
@@ -2711,46 +2711,46 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Ineffable</t>
+          <t>Contrast to Conversation</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Silence Sounds</t>
+          <t>Sounds of Silence</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Beauty</t>
+          <t>Silence</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Evolution</t>
+          <t>Alienation and Depression</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Beauty Additional</t>
+          <t>Sounds of Silence</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Beauty</t>
+          <t>Silence</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Jealousy</t>
+          <t>Ineffable</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Beauty Additional</t>
+          <t>Sounds of Silence</t>
         </is>
       </c>
     </row>
@@ -2762,12 +2762,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Brains or Beauty</t>
+          <t>Evolution</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Beauty Additional</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2779,12 +2779,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Culturally Defined:</t>
+          <t>Jealousy</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Beauty Byron</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2796,12 +2796,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Gendered</t>
+          <t>Brains or Beauty</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Beauty Byron</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -2813,12 +2813,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Beauty as Comparison</t>
+          <t>Culturally Defined:</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Beauty Byron</t>
+          <t>She Walks in Beauty</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Eyes of the Beholder</t>
+          <t>Gendered</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Beauty Flack</t>
+          <t>She Walks in Beauty</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Cosmetics, Contours and Clothes</t>
+          <t>Beauty as Comparison</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Beauty Flack</t>
+          <t>She Walks in Beauty</t>
         </is>
       </c>
     </row>
@@ -2864,12 +2864,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>More Than Just the Face</t>
+          <t>Eyes of the Beholder</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Beauty Flack</t>
+          <t>First Time Ever</t>
         </is>
       </c>
     </row>
@@ -2881,12 +2881,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Components and Composites</t>
+          <t>Cosmetics, Contours and Clothes</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Beauty Flack</t>
+          <t>First Time Ever</t>
         </is>
       </c>
     </row>
@@ -2898,12 +2898,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Beauty in Nature</t>
+          <t>More Than Just the Face</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Beauty Additional</t>
+          <t>First Time Ever</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Beauty in Man-Made Artifacts</t>
+          <t>Components and Composites</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Beauty Additional</t>
+          <t>First Time Ever</t>
         </is>
       </c>
     </row>
@@ -2932,12 +2932,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Situation Influences</t>
+          <t>Beauty in Nature</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Beauty Additional</t>
+          <t>Garden at Ste.Adresse</t>
         </is>
       </c>
     </row>
@@ -2949,12 +2949,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Physical Characteristics</t>
+          <t>Beauty in Man-Made Artifacts</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Beauty Taxi</t>
+          <t>Garden at Ste.Adresse</t>
         </is>
       </c>
     </row>
@@ -2966,12 +2966,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>La Femme Fatale</t>
+          <t>Situation Influences</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Beauty Taxi</t>
+          <t>Garden at Ste.Adresse</t>
         </is>
       </c>
     </row>
@@ -2983,12 +2983,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Different than Sexy</t>
+          <t>Physical Characteristics</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Beauty Taxi</t>
+          <t>Taxi Driver</t>
         </is>
       </c>
     </row>
@@ -3000,46 +3000,46 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Only Skin Deep</t>
+          <t>La Femme Fatale</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Beauty Taxi</t>
+          <t>Taxi Driver</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Beauty</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Survivor Guilt</t>
+          <t>Different than Sexy</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Death Addl</t>
+          <t>Taxi Driver</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Death</t>
+          <t>Beauty</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Funerals and Eulogies</t>
+          <t>Only Skin Deep</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Death Addl</t>
+          <t>Taxi Driver</t>
         </is>
       </c>
     </row>
@@ -3051,12 +3051,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Alter History</t>
+          <t>Survivor Guilt</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Death Addl</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -3068,12 +3068,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Near-Death Experiences</t>
+          <t>Funerals and Eulogies</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Death Addl</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Accidents</t>
+          <t>Alter History</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Death Bonnie</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -3102,12 +3102,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Suicide or Downhill Slide</t>
+          <t>Near-Death Experiences</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Death Bonnie</t>
+          <t>Additional</t>
         </is>
       </c>
     </row>
@@ -3119,12 +3119,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Civilian Jobs that Kill Workers</t>
+          <t>Accidents</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Death Bonnie</t>
+          <t>Bonnie &amp; Clyde</t>
         </is>
       </c>
     </row>
@@ -3136,12 +3136,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Final Physical Shut Down</t>
+          <t>Suicide or Downhill Slide</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Death Donne</t>
+          <t>Bonnie &amp; Clyde</t>
         </is>
       </c>
     </row>
@@ -3153,12 +3153,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Inevitability</t>
+          <t>Civilian Jobs that Kill Workers</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Death Donne</t>
+          <t>Bonnie &amp; Clyde</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Philosophical Pondering</t>
+          <t>Final Physical Shut Down</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Death Donne</t>
+          <t>Death be Not Proud</t>
         </is>
       </c>
     </row>
@@ -3187,12 +3187,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Courage Facing Imminent Death</t>
+          <t>Inevitability</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Death Donne</t>
+          <t>Death be Not Proud</t>
         </is>
       </c>
     </row>
@@ -3204,12 +3204,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Capital Punishment</t>
+          <t>Philosophical Pondering</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Death Hanged</t>
+          <t>Death be Not Proud</t>
         </is>
       </c>
     </row>
@@ -3221,12 +3221,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Murder</t>
+          <t>Courage Facing Imminent Death</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Death Hanged</t>
+          <t>Death be Not Proud</t>
         </is>
       </c>
     </row>
@@ -3238,12 +3238,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Mass Deaths: Wars, Pandemics, Natural Disasters</t>
+          <t>Capital Punishment</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Death Hanged</t>
+          <t>House of Hanged Man</t>
         </is>
       </c>
     </row>
@@ -3255,12 +3255,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Grief and Heartbreak</t>
+          <t>Murder</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Death Honey</t>
+          <t>House of Hanged Man</t>
         </is>
       </c>
     </row>
@@ -3272,12 +3272,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Afterlife</t>
+          <t>Mass Deaths: Wars, Pandemics, Natural Disasters</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Death Honey</t>
+          <t>House of Hanged Man</t>
         </is>
       </c>
     </row>
@@ -3289,12 +3289,896 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
+          <t>Grief and Heartbreak</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Honey</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Death</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Afterlife</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Honey</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Death</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
           <t>Religion</t>
         </is>
       </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>Death Honey</t>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Honey</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Management</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Train Wrecks</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Gare St. Lazare</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Massive Investments</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Gare St. Lazare</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Complementary Industries</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Gare St. Lazare</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Murder Orient Express</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Murder Orient Express</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Labor</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Murder Orient Express</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Train Travel</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>New Orleans</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Gale of Creative Destruction</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>New Orleans</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>New Orleans</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Government</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>New Orleans</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Formidable Power</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>The Railway Train</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Speed</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>The Railway Train</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Trains</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Metaphor of Restrictive Rails</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>The Railway Train</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Funerals and Cemeteries</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Tithing</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Prayer</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>California Dreamin'</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Clerics and Lay People</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>California Dreamin'</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Absolution and Counseling</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>California Dreamin'</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Welcoming</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>California Dreamin'</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Familiar and Reliable Support</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Dover Beach</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Ancient</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Dover Beach</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Mystical</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Dover Beach</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Defines the Proper Life</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Essoyes</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Hub of Social Life</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Essoyes</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Outreach and Serving</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Essoyes</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Honoring Deity</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Essoyes</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Sanctuary</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>On the Waterfront</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Living Properly</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>On the Waterfront</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Churches</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Privilege of Clerics</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>On the Waterfront</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Trained</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Extinct, Mythical or Cartoon</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Sayings</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Additional</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Roaming Freely</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Free Birds</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Sudden, Darting, Frightened</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Free Birds</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Pets</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Free Birds</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Flocks</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Magpie</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Migrations</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Magpie</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Feed</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Magpie</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Nests and Eggs</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Magpie</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Tuneful</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Ode to Nightingale</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Cheerful</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Ode to Nightingale</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Carefree</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Ode to Nightingale</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Pests</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>The Birds</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Hunting and Shooting</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>The Birds</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Pretty</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>The Birds</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Birds</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Symbols and Associations</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>The Birds</t>
         </is>
       </c>
     </row>

</xml_diff>